<commit_message>
Añadido las funciones del recurso Equipo
</commit_message>
<xml_diff>
--- a/api/flisol_api2.xlsx
+++ b/api/flisol_api2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
   <si>
     <t>METHOD</t>
   </si>
@@ -152,7 +152,7 @@
     <t>Lista todos los equipos con su estado actual.</t>
   </si>
   <si>
-    <t>/Equipo/documento/1117516483/tipo/cedula</t>
+    <t>/Equipo/documento/1117516483/tipo/CEDULA</t>
   </si>
   <si>
     <r>
@@ -232,18 +232,21 @@
   <si>
     <t>Agrega el estado al equipo 9 junto con sus comentarios, estos comentarios es un parametro que se envia en formato json</t>
   </si>
+  <si>
+    <t>&lt;b&gt;Warning&lt;/b&gt;:  PDOStatement::execute(): SQLSTATE[23000]: Integrity constraint violation: 1062 Duplicate entry 'REGISTRO' for key 'tipo' in &lt;b&gt;/home/infinito/www/flisol_app/api/Util/NotORM/Result.php&lt;/b&gt; on line &lt;b&gt;161&lt;/b&gt;&lt;br /&gt;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -252,6 +255,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="0"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -294,17 +303,17 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -321,6 +330,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -666,10 +678,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="4"/>
@@ -681,7 +693,7 @@
     <col min="5" max="5" width="61" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,7 +868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" ht="33" spans="1:5">
+    <row r="12" ht="49.5" spans="1:5">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -997,6 +1009,11 @@
       </c>
       <c r="E21" s="3" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="27" ht="115.5" spans="2:2">
+      <c r="B27" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>